<commit_message>
New solution for Random Forest
</commit_message>
<xml_diff>
--- a/means.xlsx
+++ b/means.xlsx
@@ -391,22 +391,22 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>0.7438747829086274</v>
+        <v>0.744136364917767</v>
       </c>
       <c r="B2">
-        <v>61.84726739798683</v>
+        <v>61.84429565824441</v>
       </c>
       <c r="C2">
-        <v>57.37534293158065</v>
+        <v>57.37533254787634</v>
       </c>
       <c r="D2">
-        <v>5.730211196403773</v>
+        <v>5.730210727470782</v>
       </c>
       <c r="E2">
-        <v>5.73236974509142</v>
+        <v>5.732369348379622</v>
       </c>
       <c r="F2">
-        <v>3.53818306568703</v>
+        <v>3.540140874333925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>